<commit_message>
cloned new additions by Marufjon in class 2/19/19
</commit_message>
<xml_diff>
--- a/src/test/resources/Countries.xlsx
+++ b/src/test/resources/Countries.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgadi\IdeaProjects\CyberTek_TestNG-Selenium-Framework\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekschool/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8897CB9-B7DC-824D-886A-A30B372522C4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" xr2:uid="{91ED3504-8F9D-994C-9701-E99A78B95D4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Country</t>
   </si>
@@ -44,7 +45,7 @@
     <t>Baku</t>
   </si>
   <si>
-    <t>Kazakhstan</t>
+    <t>Kazahstan</t>
   </si>
   <si>
     <t>Astana</t>
@@ -71,7 +72,7 @@
     <t>Russia</t>
   </si>
   <si>
-    <t>Moscow</t>
+    <t>Moskow</t>
   </si>
   <si>
     <t>Iran</t>
@@ -89,10 +90,10 @@
     <t>Tajikistan</t>
   </si>
   <si>
-    <t>Dushanbe</t>
-  </si>
-  <si>
-    <t>East Turkistan</t>
+    <t>Dushanbejanme</t>
+  </si>
+  <si>
+    <t>East Turkestan</t>
   </si>
   <si>
     <t>Urumqi</t>
@@ -104,10 +105,16 @@
     <t>Bishkek</t>
   </si>
   <si>
-    <t>Afganistan</t>
-  </si>
-  <si>
     <t>Kabul</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Mexico city</t>
   </si>
   <si>
     <t>Continent</t>
@@ -119,11 +126,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -465,20 +472,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FEC3648-E8E8-9448-9152-C17D7B392B16}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C1:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="342" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.62890625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.83984375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="13.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,10 +493,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -497,10 +504,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -508,7 +515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -516,7 +523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -524,7 +531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -532,7 +539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -540,7 +547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -548,7 +555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -556,7 +563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -564,7 +571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -572,7 +579,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -580,7 +587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -588,12 +595,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
-        <v>27</v>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>